<commit_message>
- added 8bit hex number pattern importing - cleaned up code - updated excel chart - added notes.txt - preliminary abandonment of branch - added column_printing.cpp - added (kuman) kit_example.ino
</commit_message>
<xml_diff>
--- a/pixelmapping.xlsx
+++ b/pixelmapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\source\Arduino\flappybirdhspf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417EFC30-08FE-4909-8D5C-387B8CD80980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5061E73E-6B7C-47B8-A441-17185E4FEB44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{7FF34EEA-2A7E-4622-AD68-76FEE56603D3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="9">
   <si>
     <t>0x00</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>0 0 1 0 1 1 0 0</t>
+  </si>
+  <si>
+    <t>Referenz 8-Bit</t>
   </si>
 </sst>
 </file>
@@ -434,21 +437,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB2203F9-49A3-439E-BAD1-10BB3B99AEF0}">
-  <dimension ref="D1:O12"/>
+  <dimension ref="D1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T31" sqref="T31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="7.88671875" customWidth="1"/>
-    <col min="9" max="9" width="6.88671875" customWidth="1"/>
-    <col min="10" max="10" width="7.21875" customWidth="1"/>
-    <col min="11" max="11" width="7.109375" customWidth="1"/>
-    <col min="12" max="12" width="6.88671875" customWidth="1"/>
-    <col min="13" max="13" width="8.109375" customWidth="1"/>
-    <col min="14" max="14" width="7.109375" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.21875" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" customWidth="1"/>
+    <col min="8" max="15" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="24" width="6.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="4:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -577,6 +579,53 @@
     <row r="12" spans="4:15" x14ac:dyDescent="0.3">
       <c r="H12" s="3"/>
     </row>
+    <row r="18" spans="7:16" x14ac:dyDescent="0.3">
+      <c r="H18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="P18" s="2"/>
+    </row>
+    <row r="19" spans="7:16" x14ac:dyDescent="0.3">
+      <c r="H19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="N19" s="2"/>
+    </row>
+    <row r="20" spans="7:16" x14ac:dyDescent="0.3">
+      <c r="G20" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="L20" s="2"/>
+    </row>
+    <row r="21" spans="7:16" x14ac:dyDescent="0.3">
+      <c r="H21" s="2"/>
+      <c r="J21" s="2"/>
+    </row>
+    <row r="22" spans="7:16" x14ac:dyDescent="0.3">
+      <c r="H22" s="2"/>
+      <c r="P22" s="2"/>
+    </row>
+    <row r="23" spans="7:16" x14ac:dyDescent="0.3">
+      <c r="H23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="P23" s="2"/>
+    </row>
+    <row r="24" spans="7:16" x14ac:dyDescent="0.3">
+      <c r="H24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="P24" s="2"/>
+    </row>
+    <row r="25" spans="7:16" x14ac:dyDescent="0.3">
+      <c r="H25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="P25" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>